<commit_message>
New FDO DAVID BP
</commit_message>
<xml_diff>
--- a/output/Func_annot_DAVID/FDO_BP_DAVID.xlsx
+++ b/output/Func_annot_DAVID/FDO_BP_DAVID.xlsx
@@ -1,69 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10329"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/graceleuchtenberger/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{384ECDB0-0CAC-9B40-83C1-C556CFCC7E9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B032EE3A-8D69-7D4C-9801-18F35D1FBFEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5180" yWindow="1800" windowWidth="28040" windowHeight="17440" xr2:uid="{1AE02A18-3D99-7241-A405-3D513411E137}"/>
+    <workbookView xWindow="660" yWindow="540" windowWidth="28040" windowHeight="17440" xr2:uid="{3AB9D2C1-8C40-9641-B27B-778552B746C0}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="FDO_DAVID_chart" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="FDO_BP_DAVID" localSheetId="0">Sheet1!$A$1:$M$37</definedName>
-  </definedNames>
-  <calcPr calcId="181029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
-<file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
-  <connection id="1" xr16:uid="{C5D449BF-7AA1-8547-8091-D87803F16F56}" name="FDO_BP_DAVID" type="6" refreshedVersion="8" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/graceleuchtenberger/Desktop/FDO_BP_DAVID">
-      <textFields count="13">
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-      </textFields>
-    </textPr>
-  </connection>
-</connections>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="102">
   <si>
     <t>Category</t>
   </si>
@@ -101,7 +58,7 @@
     <t>Benjamini</t>
   </si>
   <si>
-    <t>FDR</t>
+    <t>FDR\</t>
   </si>
   <si>
     <t>GOTERM_BP_DIRECT</t>
@@ -110,7 +67,37 @@
     <t>GO:0060294~cilium movement involved in cell motility</t>
   </si>
   <si>
-    <t>Q8TE73, O95995, Q8WXX0, P0C6F1, A6H782, Q8TD57, Q8IWG1</t>
+    <t>Q8TE73, O95995, Q63170, Q8WXX0, P0C6F1, A6H782, Q39565, Q8TD57, Q8IWG1</t>
+  </si>
+  <si>
+    <t>7.410533589184669E-4\</t>
+  </si>
+  <si>
+    <t>GO:0003341~cilium movement</t>
+  </si>
+  <si>
+    <t>Q8TE73, Q0V9R4, Q4R8V8, Q63170, A8CVX7, Q8WXX0, Q4G0P3, P0C6F1, Q61371, B5X5D0</t>
+  </si>
+  <si>
+    <t>0.006441210732561733\</t>
+  </si>
+  <si>
+    <t>GO:0036159~inner dynein arm assembly</t>
+  </si>
+  <si>
+    <t>Q0V9R4, Q4R8V8, Q63170, Q8WXX0, P0C6F1, Q8IWG1</t>
+  </si>
+  <si>
+    <t>0.009370040594647449\</t>
+  </si>
+  <si>
+    <t>GO:0000226~microtubule cytoskeleton organization</t>
+  </si>
+  <si>
+    <t>P06603, Q86XH1, Q68FR8, A8CVX7, Q96MT7, F7E540, O75410, Q80UG8, P68372, P02554, Q8CHB8</t>
+  </si>
+  <si>
+    <t>0.009770169675682346\</t>
   </si>
   <si>
     <t>GO:0003333~amino acid transmembrane transport</t>
@@ -119,16 +106,22 @@
     <t>Q9N1R6, P31646, Q5RAE3, Q01650</t>
   </si>
   <si>
+    <t>0.03274635111967198\</t>
+  </si>
+  <si>
     <t>GO:0015804~neutral amino acid transport</t>
   </si>
   <si>
     <t>Q9N1R6, Q5RAE3, Q01650, Q9H1V8</t>
   </si>
   <si>
-    <t>GO:0000226~microtubule cytoskeleton organization</t>
-  </si>
-  <si>
-    <t>P06603, Q68FR8, A8CVX7, Q96MT7, F7E540, Q80UG8, P68372, P02554, Q8CHB8</t>
+    <t>GO:0006542~glutamine biosynthetic process</t>
+  </si>
+  <si>
+    <t>Q8HZM5</t>
+  </si>
+  <si>
+    <t>0.04275231229691412\</t>
   </si>
   <si>
     <t>GO:0060285~cilium-dependent cell motility</t>
@@ -137,16 +130,34 @@
     <t>Q0V9R4, Q8WXX0, P0C6F1, Q7T0Y4, Q8TD57</t>
   </si>
   <si>
-    <t>GO:0003341~cilium movement</t>
-  </si>
-  <si>
-    <t>Q8TE73, Q0V9R4, Q4R8V8, A8CVX7, Q8WXX0, Q4G0P3, P0C6F1, B5X5D0</t>
-  </si>
-  <si>
-    <t>GO:0036159~inner dynein arm assembly</t>
-  </si>
-  <si>
-    <t>Q0V9R4, Q4R8V8, Q8WXX0, P0C6F1, Q8IWG1</t>
+    <t>GO:1904749~regulation of protein localization to nucleolus</t>
+  </si>
+  <si>
+    <t>0.08058675580762788\</t>
+  </si>
+  <si>
+    <t>GO:0010594~regulation of endothelial cell migration</t>
+  </si>
+  <si>
+    <t>0.14055381160325622\</t>
+  </si>
+  <si>
+    <t>GO:0007018~microtubule-based movement</t>
+  </si>
+  <si>
+    <t>Q8TE73, F8WLE0, Q63170, P0C6F1, Q39565, Q7XPJ0, Q8TD57, Q9D5I4</t>
+  </si>
+  <si>
+    <t>0.23509347806145292\</t>
+  </si>
+  <si>
+    <t>GO:0018345~protein palmitoylation</t>
+  </si>
+  <si>
+    <t>0.26397962829125204\</t>
+  </si>
+  <si>
+    <t>GO:1903670~regulation of sprouting angiogenesis</t>
   </si>
   <si>
     <t>GO:0018095~protein polyglutamylation</t>
@@ -161,16 +172,40 @@
     <t>Q9N1R6, Q64319</t>
   </si>
   <si>
+    <t>0.3599029257781063\</t>
+  </si>
+  <si>
+    <t>GO:0007288~sperm axoneme assembly</t>
+  </si>
+  <si>
+    <t>Q2IA00, Q96MT7, Q61371, Q4R7Y8, Q8CHB8</t>
+  </si>
+  <si>
+    <t>0.9022215102220053\</t>
+  </si>
+  <si>
+    <t>GO:0030317~flagellated sperm motility</t>
+  </si>
+  <si>
+    <t>Q8TE73, Q2YDN4, E1BJL9, O95995, P68372, A6H782, Q4R7Y8, Q8CHB8</t>
+  </si>
+  <si>
+    <t>GO:0035082~axoneme assembly</t>
+  </si>
+  <si>
+    <t>O95995, A8CVX7, Q3V0L5, Q7T0Y4, B5X5D0</t>
+  </si>
+  <si>
+    <t>0.9753282034049445\</t>
+  </si>
+  <si>
     <t>GO:0007017~microtubule-based process</t>
   </si>
   <si>
     <t>P06603, Q68FR8, P68372</t>
   </si>
   <si>
-    <t>GO:0030317~flagellated sperm motility</t>
-  </si>
-  <si>
-    <t>Q8TE73, O95995, A6H782, Q3V2A7, Q4R7Y8, Q8CHB8</t>
+    <t>0.9943074003795066\</t>
   </si>
   <si>
     <t>GO:0036211~protein modification process</t>
@@ -179,10 +214,10 @@
     <t>A8CVX7, F7E540, Q80UG8, Q9Y572, Q8CHB8</t>
   </si>
   <si>
-    <t>GO:0006816~calcium ion transport</t>
-  </si>
-  <si>
-    <t>Q9VDG5, Q02485, P11881, Q9Z0J4, Q91WD2</t>
+    <t>GO:0008283~cell population proliferation</t>
+  </si>
+  <si>
+    <t>O75410, Q9D4C1, P62325, Q8HZM5</t>
   </si>
   <si>
     <t>GO:0032729~positive regulation of type II interferon production</t>
@@ -191,28 +226,37 @@
     <t>P14270, Q01650, Q5ZL72</t>
   </si>
   <si>
-    <t>GO:0002376~immune system process</t>
-  </si>
-  <si>
-    <t>P17710, Q8R151, Q5RHR0, Q8R5F7, Q98925, E9Q555</t>
-  </si>
-  <si>
-    <t>GO:0051209~release of sequestered calcium ion into cytosol</t>
-  </si>
-  <si>
-    <t>Q32NH8, Q9TU34, Q02485, P11881</t>
-  </si>
-  <si>
-    <t>GO:0098703~calcium ion import across plasma membrane</t>
-  </si>
-  <si>
-    <t>Q9VDG5, Q02485, Q91WD2</t>
-  </si>
-  <si>
-    <t>GO:0035082~axoneme assembly</t>
-  </si>
-  <si>
-    <t>O95995, A8CVX7, Q3V0L5, B5X5D0</t>
+    <t>GO:0000278~mitotic cell cycle</t>
+  </si>
+  <si>
+    <t>Q9DBR7, P06603, Q68FR8, P68372, P02554</t>
+  </si>
+  <si>
+    <t>GO:0009267~cellular response to starvation</t>
+  </si>
+  <si>
+    <t>Q9BXW4, Q8HZM5</t>
+  </si>
+  <si>
+    <t>GO:0007420~brain development</t>
+  </si>
+  <si>
+    <t>O95995, Q80Y17, P78509, Q61371, P40656, Q9H1V8, Q864U8</t>
+  </si>
+  <si>
+    <t>GO:0007417~central nervous system development</t>
+  </si>
+  <si>
+    <t>P20303, Q86XL3, P78509, P80206, Q864U8</t>
+  </si>
+  <si>
+    <t>GO:0042254~ribosome biogenesis</t>
+  </si>
+  <si>
+    <t>Q13823, Q5XGY1, Q8HZM5</t>
+  </si>
+  <si>
+    <t>GO:0009749~response to glucose</t>
   </si>
   <si>
     <t>GO:0033137~negative regulation of peptidyl-serine phosphorylation</t>
@@ -221,10 +265,10 @@
     <t>Q16611, P14270, Q9Z0J4</t>
   </si>
   <si>
-    <t>GO:0007288~sperm axoneme assembly</t>
-  </si>
-  <si>
-    <t>Q96MT7, Q0VFN8, Q4R7Y8, Q8CHB8</t>
+    <t>GO:0070286~axonemal dynein complex assembly</t>
+  </si>
+  <si>
+    <t>Q0V9R4, Q9D180, Q7T0Y4</t>
   </si>
   <si>
     <t>GO:0050767~regulation of neurogenesis</t>
@@ -233,95 +277,62 @@
     <t>Q90Z12, Q9VGZ5, Q9Z0J4</t>
   </si>
   <si>
+    <t>GO:0065003~protein-containing complex assembly</t>
+  </si>
+  <si>
+    <t>Q80Y17, P20303, P14270, Q7T0Y4, P80206</t>
+  </si>
+  <si>
+    <t>GO:0089718~amino acid import across plasma membrane</t>
+  </si>
+  <si>
+    <t>P31646, Q01650</t>
+  </si>
+  <si>
+    <t>GO:1903514~release of sequestered calcium ion into cytosol by endoplasmic reticulum</t>
+  </si>
+  <si>
+    <t>Q9TU34, P11881</t>
+  </si>
+  <si>
+    <t>GO:0015820~L-leucine transport</t>
+  </si>
+  <si>
+    <t>Q01650, Q9H1V8</t>
+  </si>
+  <si>
+    <t>GO:0015824~proline transport</t>
+  </si>
+  <si>
+    <t>GO:0032328~alanine transport</t>
+  </si>
+  <si>
+    <t>GO:0002720~positive regulation of cytokine production involved in immune response</t>
+  </si>
+  <si>
+    <t>P17710, Q01650</t>
+  </si>
+  <si>
+    <t>GO:0008306~associative learning</t>
+  </si>
+  <si>
+    <t>P78509, Q3KN41, P17971</t>
+  </si>
+  <si>
     <t>GO:0009952~anterior/posterior pattern specification</t>
   </si>
   <si>
-    <t>Q90Z12, Q9VGZ5, Q8N2E2, P80206</t>
-  </si>
-  <si>
-    <t>GO:0007018~microtubule-based movement</t>
-  </si>
-  <si>
-    <t>Q8TE73, B1AVY7, P0C6F1, Q8TD57, Q9D5I4</t>
-  </si>
-  <si>
-    <t>GO:0015824~proline transport</t>
-  </si>
-  <si>
-    <t>Q01650, Q9H1V8</t>
-  </si>
-  <si>
-    <t>GO:0015820~L-leucine transport</t>
-  </si>
-  <si>
-    <t>GO:0002720~positive regulation of cytokine production involved in immune response</t>
-  </si>
-  <si>
-    <t>P17710, Q01650</t>
-  </si>
-  <si>
-    <t>GO:0089718~amino acid import across plasma membrane</t>
-  </si>
-  <si>
-    <t>P31646, Q01650</t>
-  </si>
-  <si>
-    <t>GO:0032328~alanine transport</t>
-  </si>
-  <si>
-    <t>GO:0035725~sodium ion transmembrane transport</t>
-  </si>
-  <si>
-    <t>P31646, Q9VDG5, Q9JIH7, Q9H1V8</t>
-  </si>
-  <si>
-    <t>GO:0150104~transport across blood-brain barrier</t>
-  </si>
-  <si>
-    <t>P20303, Q01650, Q9H1V8</t>
-  </si>
-  <si>
-    <t>GO:0070059~intrinsic apoptotic signaling pathway in response to endoplasmic reticulum stress</t>
-  </si>
-  <si>
-    <t>Q16611, Q9TU34, P11881</t>
-  </si>
-  <si>
-    <t>GO:0000278~mitotic cell cycle</t>
-  </si>
-  <si>
-    <t>P06603, Q68FR8, P68372, P02554</t>
-  </si>
-  <si>
-    <t>GO:0036098~male germ-line stem cell population maintenance</t>
-  </si>
-  <si>
-    <t>Q68FR8</t>
-  </si>
-  <si>
-    <t>GO:0051344~negative regulation of cyclic-nucleotide phosphodiesterase activity</t>
-  </si>
-  <si>
-    <t>Q15043, P59722</t>
-  </si>
-  <si>
-    <t>GO:0070327~thyroid hormone transport</t>
-  </si>
-  <si>
-    <t>Q5RAE3, Q01650</t>
-  </si>
-  <si>
-    <t>GO:0070588~calcium ion transmembrane transport</t>
-  </si>
-  <si>
-    <t>Q9TU34, Q02485, P11881, Q91WD2</t>
+    <t>Q90Z12, Q9VGZ5, Q61371, P80206</t>
+  </si>
+  <si>
+    <t>0.9943074003795066}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -329,16 +340,316 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Aptos Display"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF006100"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C0006"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C5700"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -346,16 +657,205 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="42">
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -368,10 +868,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="FDO_BP_DAVID" connectionId="1" xr16:uid="{17264388-65A4-C747-A300-8912A26F9807}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -690,23 +1186,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{125BC1AD-2821-F049-8339-01DB2DFE3759}">
-  <dimension ref="A1:M37"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7448C2C-E82C-1E47-BFE2-CE209A512AC3}">
+  <dimension ref="A1:M41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="79.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="67" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.83203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="13" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.5" customWidth="1"/>
+    <col min="2" max="2" width="72.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
@@ -758,37 +1248,37 @@
         <v>14</v>
       </c>
       <c r="C2">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D2">
-        <v>3.2558139534883699</v>
+        <v>3.4351145038167901</v>
       </c>
       <c r="E2" s="1">
-        <v>3.6136362436776603E-5</v>
+        <v>7.0711198370082704E-7</v>
       </c>
       <c r="F2" t="s">
         <v>15</v>
       </c>
       <c r="G2">
-        <v>172</v>
+        <v>213</v>
       </c>
       <c r="H2">
         <v>20</v>
       </c>
       <c r="I2">
-        <v>5048</v>
+        <v>5033</v>
       </c>
       <c r="J2">
-        <v>10.272093023255801</v>
-      </c>
-      <c r="K2">
-        <v>3.0529816406188699E-2</v>
-      </c>
-      <c r="L2">
-        <v>2.26245882356018E-2</v>
-      </c>
-      <c r="M2">
-        <v>2.25191122997715E-2</v>
+        <v>10.633098591549199</v>
+      </c>
+      <c r="K2" s="1">
+        <v>7.4572521524440805E-4</v>
+      </c>
+      <c r="L2" s="1">
+        <v>7.4600314280437203E-4</v>
+      </c>
+      <c r="M2" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
@@ -796,40 +1286,40 @@
         <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C3">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D3">
-        <v>2.3255813953488298</v>
+        <v>3.8167938931297698</v>
       </c>
       <c r="E3" s="1">
-        <v>8.0022893396357504E-5</v>
+        <v>1.2292386894201699E-5</v>
       </c>
       <c r="F3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G3">
-        <v>172</v>
+        <v>213</v>
       </c>
       <c r="H3">
-        <v>8</v>
+        <v>36</v>
       </c>
       <c r="I3">
-        <v>5048</v>
+        <v>5033</v>
       </c>
       <c r="J3">
-        <v>18.3430232558139</v>
+        <v>6.5636411058946198</v>
       </c>
       <c r="K3">
-        <v>6.6358166166905805E-2</v>
+        <v>1.28848186035024E-2</v>
       </c>
       <c r="L3">
-        <v>2.26245882356018E-2</v>
-      </c>
-      <c r="M3">
-        <v>2.25191122997715E-2</v>
+        <v>6.4842340866914303E-3</v>
+      </c>
+      <c r="M3" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
@@ -837,40 +1327,40 @@
         <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C4">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D4">
-        <v>2.3255813953488298</v>
+        <v>2.2900763358778602</v>
       </c>
       <c r="E4" s="1">
-        <v>8.0022893396357504E-5</v>
+        <v>2.6822635290021302E-5</v>
       </c>
       <c r="F4" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="G4">
-        <v>172</v>
+        <v>213</v>
       </c>
       <c r="H4">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="I4">
-        <v>5048</v>
+        <v>5033</v>
       </c>
       <c r="J4">
-        <v>18.3430232558139</v>
+        <v>14.1774647887323</v>
       </c>
       <c r="K4">
-        <v>6.6358166166905805E-2</v>
+        <v>2.7901614262525201E-2</v>
       </c>
       <c r="L4">
-        <v>2.26245882356018E-2</v>
-      </c>
-      <c r="M4">
-        <v>2.25191122997715E-2</v>
+        <v>9.4326267436574997E-3</v>
+      </c>
+      <c r="M4" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
@@ -878,40 +1368,40 @@
         <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C5">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D5">
-        <v>4.6511627906976702</v>
+        <v>4.5801526717557204</v>
       </c>
       <c r="E5" s="1">
-        <v>1.0547593583031101E-4</v>
+        <v>3.7290723952986003E-5</v>
       </c>
       <c r="F5" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="G5">
-        <v>172</v>
+        <v>213</v>
       </c>
       <c r="H5">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="I5">
-        <v>5048</v>
+        <v>5033</v>
       </c>
       <c r="J5">
-        <v>5.1489188086495297</v>
+        <v>4.6483491110598001</v>
       </c>
       <c r="K5">
-        <v>8.6528521594598895E-2</v>
+        <v>3.8578583429360797E-2</v>
       </c>
       <c r="L5">
-        <v>2.26245882356018E-2</v>
-      </c>
-      <c r="M5">
-        <v>2.25191122997715E-2</v>
+        <v>9.8354284426000697E-3</v>
+      </c>
+      <c r="M5" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
@@ -919,40 +1409,40 @@
         <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C6">
         <v>5</v>
       </c>
       <c r="D6">
-        <v>2.3255813953488298</v>
+        <v>1.90839694656488</v>
       </c>
       <c r="E6" s="1">
-        <v>2.2757450409642701E-4</v>
+        <v>1.8747910946377E-4</v>
       </c>
       <c r="F6" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="G6">
-        <v>172</v>
+        <v>213</v>
       </c>
       <c r="H6">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="I6">
-        <v>5048</v>
+        <v>5033</v>
       </c>
       <c r="J6">
-        <v>14.6744186046511</v>
+        <v>14.768192488262899</v>
       </c>
       <c r="K6">
-        <v>0.17739664598705501</v>
+        <v>0.17947344420238701</v>
       </c>
       <c r="L6">
-        <v>3.9051784902946897E-2</v>
-      </c>
-      <c r="M6">
-        <v>3.88697252996697E-2</v>
+        <v>3.2965076747379703E-2</v>
+      </c>
+      <c r="M6" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
@@ -960,40 +1450,40 @@
         <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="C7">
+        <v>5</v>
+      </c>
+      <c r="D7">
+        <v>1.90839694656488</v>
+      </c>
+      <c r="E7" s="1">
+        <v>1.8747910946377E-4</v>
+      </c>
+      <c r="F7" t="s">
+        <v>30</v>
+      </c>
+      <c r="G7">
+        <v>213</v>
+      </c>
+      <c r="H7">
         <v>8</v>
       </c>
-      <c r="D7">
-        <v>3.7209302325581302</v>
-      </c>
-      <c r="E7" s="1">
-        <v>2.7832872283998198E-4</v>
-      </c>
-      <c r="F7" t="s">
-        <v>25</v>
-      </c>
-      <c r="G7">
-        <v>172</v>
-      </c>
-      <c r="H7">
-        <v>39</v>
-      </c>
       <c r="I7">
-        <v>5048</v>
+        <v>5033</v>
       </c>
       <c r="J7">
-        <v>6.0202742993440603</v>
+        <v>14.768192488262899</v>
       </c>
       <c r="K7">
-        <v>0.212458557015611</v>
+        <v>0.17947344420238701</v>
       </c>
       <c r="L7">
-        <v>3.98010073661174E-2</v>
-      </c>
-      <c r="M7">
-        <v>3.9615454884224098E-2</v>
+        <v>3.2965076747379703E-2</v>
+      </c>
+      <c r="M7" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
@@ -1001,40 +1491,40 @@
         <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="C8">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D8">
-        <v>2.3255813953488298</v>
+        <v>1.5267175572519001</v>
       </c>
       <c r="E8" s="1">
-        <v>5.0856352112862502E-4</v>
+        <v>2.8571064955180199E-4</v>
       </c>
       <c r="F8" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="G8">
-        <v>172</v>
+        <v>213</v>
       </c>
       <c r="H8">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="I8">
-        <v>5048</v>
+        <v>5033</v>
       </c>
       <c r="J8">
-        <v>12.2286821705426</v>
+        <v>23.629107981220599</v>
       </c>
       <c r="K8">
-        <v>0.35367867643955597</v>
+        <v>0.26026835733973702</v>
       </c>
       <c r="L8">
-        <v>6.23353573040515E-2</v>
-      </c>
-      <c r="M8">
-        <v>6.20447495776923E-2</v>
+        <v>4.3037871634775099E-2</v>
+      </c>
+      <c r="M8" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
@@ -1042,40 +1532,40 @@
         <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="C9">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D9">
-        <v>1.86046511627906</v>
-      </c>
-      <c r="E9">
-        <v>2.7597272103312099E-3</v>
+        <v>1.90839694656488</v>
+      </c>
+      <c r="E9" s="1">
+        <v>3.2635352898407701E-4</v>
       </c>
       <c r="F9" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="G9">
-        <v>172</v>
+        <v>213</v>
       </c>
       <c r="H9">
         <v>9</v>
       </c>
       <c r="I9">
-        <v>5048</v>
+        <v>5033</v>
       </c>
       <c r="J9">
-        <v>13.0439276485788</v>
+        <v>13.127282211789201</v>
       </c>
       <c r="K9">
-        <v>0.90662384579334099</v>
+        <v>0.29132565049565001</v>
       </c>
       <c r="L9">
-        <v>0.29598074330802199</v>
-      </c>
-      <c r="M9">
-        <v>0.29460087970285598</v>
+        <v>4.3037871634775099E-2</v>
+      </c>
+      <c r="M9" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
@@ -1083,40 +1573,40 @@
         <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="C10">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D10">
-        <v>1.3953488372092999</v>
-      </c>
-      <c r="E10">
-        <v>3.3466234512300901E-3</v>
+        <v>1.5267175572519001</v>
+      </c>
+      <c r="E10" s="1">
+        <v>6.9206183422581104E-4</v>
       </c>
       <c r="F10" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G10">
-        <v>172</v>
+        <v>213</v>
       </c>
       <c r="H10">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I10">
-        <v>5048</v>
+        <v>5033</v>
       </c>
       <c r="J10">
-        <v>29.3488372093023</v>
+        <v>18.9032863849765</v>
       </c>
       <c r="K10">
-        <v>0.94365255719581498</v>
+        <v>0.51827313594592195</v>
       </c>
       <c r="L10">
-        <v>0.31904476901726803</v>
-      </c>
-      <c r="M10">
-        <v>0.31755738081672202</v>
+        <v>8.1125026123136795E-2</v>
+      </c>
+      <c r="M10" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
@@ -1124,40 +1614,40 @@
         <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="C11">
         <v>4</v>
       </c>
       <c r="D11">
-        <v>1.86046511627906</v>
+        <v>1.5267175572519001</v>
       </c>
       <c r="E11">
-        <v>8.5024678410334092E-3</v>
+        <v>1.34116232445855E-3</v>
       </c>
       <c r="F11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G11">
-        <v>172</v>
+        <v>213</v>
       </c>
       <c r="H11">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="I11">
-        <v>5048</v>
+        <v>5033</v>
       </c>
       <c r="J11">
-        <v>9.0304114490160998</v>
+        <v>15.7527386541471</v>
       </c>
       <c r="K11">
-        <v>0.999342001285076</v>
+        <v>0.75728707785889804</v>
       </c>
       <c r="L11">
-        <v>0.72951174076066705</v>
-      </c>
-      <c r="M11">
-        <v>0.72611075362425304</v>
+        <v>0.14149262523037701</v>
+      </c>
+      <c r="M11" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
@@ -1165,40 +1655,40 @@
         <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="C12">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D12">
-        <v>2.7906976744185998</v>
+        <v>3.0534351145038099</v>
       </c>
       <c r="E12">
-        <v>9.5264108950244494E-3</v>
+        <v>2.4675842162938701E-3</v>
       </c>
       <c r="F12" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="G12">
-        <v>172</v>
+        <v>213</v>
       </c>
       <c r="H12">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="I12">
-        <v>5048</v>
+        <v>5033</v>
       </c>
       <c r="J12">
-        <v>4.5152057245080499</v>
+        <v>4.2007303077725604</v>
       </c>
       <c r="K12">
-        <v>0.99972885109217702</v>
+        <v>0.92620900504909598</v>
       </c>
       <c r="L12">
-        <v>0.74306004981190699</v>
-      </c>
-      <c r="M12">
-        <v>0.73959590039553502</v>
+        <v>0.23666375892636701</v>
+      </c>
+      <c r="M12" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
@@ -1206,40 +1696,40 @@
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="C13">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D13">
-        <v>2.3255813953488298</v>
+        <v>1.5267175572519001</v>
       </c>
       <c r="E13">
-        <v>1.06077884826192E-2</v>
+        <v>3.5264454161045098E-3</v>
       </c>
       <c r="F13" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="G13">
-        <v>172</v>
+        <v>213</v>
       </c>
       <c r="H13">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="I13">
-        <v>5048</v>
+        <v>5033</v>
       </c>
       <c r="J13">
-        <v>5.6440071556350597</v>
+        <v>11.8145539906103</v>
       </c>
       <c r="K13">
-        <v>0.99989379081233098</v>
+        <v>0.97593448246096604</v>
       </c>
       <c r="L13">
-        <v>0.758456876507278</v>
-      </c>
-      <c r="M13">
-        <v>0.754920947013072</v>
+        <v>0.265742850999304</v>
+      </c>
+      <c r="M13" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
@@ -1247,40 +1737,40 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="C14">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D14">
-        <v>2.3255813953488298</v>
+        <v>1.5267175572519001</v>
       </c>
       <c r="E14">
-        <v>1.75127089174579E-2</v>
+        <v>3.5264454161045098E-3</v>
       </c>
       <c r="F14" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="G14">
-        <v>172</v>
+        <v>213</v>
       </c>
       <c r="H14">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="I14">
-        <v>5048</v>
+        <v>5033</v>
       </c>
       <c r="J14">
-        <v>4.8914728682170496</v>
+        <v>11.8145539906103</v>
       </c>
       <c r="K14">
-        <v>0.99999973907504003</v>
+        <v>0.97593448246096604</v>
       </c>
       <c r="L14">
-        <v>1</v>
-      </c>
-      <c r="M14">
-        <v>0.99649941656942798</v>
+        <v>0.265742850999304</v>
+      </c>
+      <c r="M14" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
@@ -1288,40 +1778,40 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="C15">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D15">
-        <v>1.3953488372092999</v>
+        <v>1.5267175572519001</v>
       </c>
       <c r="E15">
-        <v>2.1416462558288898E-2</v>
+        <v>3.5264454161045098E-3</v>
       </c>
       <c r="F15" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="G15">
-        <v>172</v>
+        <v>213</v>
       </c>
       <c r="H15">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I15">
-        <v>5048</v>
+        <v>5033</v>
       </c>
       <c r="J15">
-        <v>12.578073089700901</v>
+        <v>11.8145539906103</v>
       </c>
       <c r="K15">
-        <v>0.99999999142956497</v>
+        <v>0.97593448246096604</v>
       </c>
       <c r="L15">
-        <v>1</v>
-      </c>
-      <c r="M15">
-        <v>0.99649941656942798</v>
+        <v>0.265742850999304</v>
+      </c>
+      <c r="M15" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
@@ -1329,40 +1819,40 @@
         <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="C16">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D16">
-        <v>2.7906976744185998</v>
+        <v>1.1450381679389301</v>
       </c>
       <c r="E16">
-        <v>2.2215300623874501E-2</v>
+        <v>5.1512823346102996E-3</v>
       </c>
       <c r="F16" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="G16">
-        <v>172</v>
+        <v>213</v>
       </c>
       <c r="H16">
-        <v>48</v>
+        <v>3</v>
       </c>
       <c r="I16">
-        <v>5048</v>
+        <v>5033</v>
       </c>
       <c r="J16">
-        <v>3.6686046511627901</v>
+        <v>23.629107981220599</v>
       </c>
       <c r="K16">
-        <v>0.99999999574697995</v>
+        <v>0.99569788581726804</v>
       </c>
       <c r="L16">
-        <v>1</v>
-      </c>
-      <c r="M16">
-        <v>0.99649941656942798</v>
+        <v>0.36230685753425701</v>
+      </c>
+      <c r="M16" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
@@ -1370,40 +1860,40 @@
         <v>13</v>
       </c>
       <c r="B17" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="C17">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D17">
-        <v>1.86046511627906</v>
+        <v>1.90839694656488</v>
       </c>
       <c r="E17">
-        <v>2.4828094401061401E-2</v>
+        <v>1.4424732762237699E-2</v>
       </c>
       <c r="F17" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="G17">
-        <v>172</v>
+        <v>213</v>
       </c>
       <c r="H17">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="I17">
-        <v>5048</v>
+        <v>5033</v>
       </c>
       <c r="J17">
-        <v>6.1787025703794303</v>
+        <v>5.13676260461318</v>
       </c>
       <c r="K17">
-        <v>0.99999999957179297</v>
+        <v>0.99999977984160404</v>
       </c>
       <c r="L17">
-        <v>1</v>
-      </c>
-      <c r="M17">
-        <v>0.99649941656942798</v>
+        <v>0.90824779893532004</v>
+      </c>
+      <c r="M17" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.2">
@@ -1411,40 +1901,40 @@
         <v>13</v>
       </c>
       <c r="B18" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="C18">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="D18">
-        <v>1.3953488372092999</v>
+        <v>3.0534351145038099</v>
       </c>
       <c r="E18">
-        <v>3.5116914412800897E-2</v>
+        <v>1.4635272589479E-2</v>
       </c>
       <c r="F18" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="G18">
-        <v>172</v>
+        <v>213</v>
       </c>
       <c r="H18">
-        <v>9</v>
+        <v>62</v>
       </c>
       <c r="I18">
-        <v>5048</v>
+        <v>5033</v>
       </c>
       <c r="J18">
-        <v>9.7829457364340993</v>
+        <v>3.0489171588671802</v>
       </c>
       <c r="K18">
-        <v>0.99999999999995204</v>
+        <v>0.99999982426929002</v>
       </c>
       <c r="L18">
-        <v>1</v>
-      </c>
-      <c r="M18">
-        <v>0.99649941656942798</v>
+        <v>0.90824779893532004</v>
+      </c>
+      <c r="M18" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
@@ -1452,40 +1942,40 @@
         <v>13</v>
       </c>
       <c r="B19" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="C19">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D19">
-        <v>1.86046511627906</v>
+        <v>1.90839694656488</v>
       </c>
       <c r="E19">
-        <v>3.6653578443377098E-2</v>
+        <v>1.6751820287489502E-2</v>
       </c>
       <c r="F19" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="G19">
-        <v>172</v>
+        <v>213</v>
       </c>
       <c r="H19">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="I19">
-        <v>5048</v>
+        <v>5033</v>
       </c>
       <c r="J19">
-        <v>5.3361522198731501</v>
+        <v>4.9227308294209697</v>
       </c>
       <c r="K19">
-        <v>0.99999999999998701</v>
+        <v>0.99999998181872296</v>
       </c>
       <c r="L19">
-        <v>1</v>
-      </c>
-      <c r="M19">
-        <v>0.99649941656942798</v>
+        <v>0.98184280018341197</v>
+      </c>
+      <c r="M19" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
@@ -1493,40 +1983,40 @@
         <v>13</v>
       </c>
       <c r="B20" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="C20">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D20">
-        <v>1.3953488372092999</v>
+        <v>1.5267175572519001</v>
       </c>
       <c r="E20">
-        <v>4.2934909137548598E-2</v>
+        <v>1.9012522939543301E-2</v>
       </c>
       <c r="F20" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="G20">
-        <v>172</v>
+        <v>213</v>
       </c>
       <c r="H20">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="I20">
-        <v>5048</v>
+        <v>5033</v>
       </c>
       <c r="J20">
-        <v>8.8046511627906892</v>
+        <v>6.75117370892018</v>
       </c>
       <c r="K20">
-        <v>1</v>
+        <v>0.99999999839692499</v>
       </c>
       <c r="L20">
         <v>1</v>
       </c>
-      <c r="M20">
-        <v>0.99649941656942798</v>
+      <c r="M20" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.2">
@@ -1534,40 +2024,40 @@
         <v>13</v>
       </c>
       <c r="B21" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="C21">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D21">
-        <v>1.86046511627906</v>
+        <v>1.90839694656488</v>
       </c>
       <c r="E21">
-        <v>4.5872647192264297E-2</v>
+        <v>1.9300911285516899E-2</v>
       </c>
       <c r="F21" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="G21">
-        <v>172</v>
+        <v>213</v>
       </c>
       <c r="H21">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I21">
-        <v>5048</v>
+        <v>5033</v>
       </c>
       <c r="J21">
-        <v>4.8914728682170496</v>
+        <v>4.7258215962441303</v>
       </c>
       <c r="K21">
-        <v>1</v>
+        <v>0.99999999882445501</v>
       </c>
       <c r="L21">
         <v>1</v>
       </c>
-      <c r="M21">
-        <v>0.99649941656942798</v>
+      <c r="M21" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.2">
@@ -1575,40 +2065,40 @@
         <v>13</v>
       </c>
       <c r="B22" t="s">
+        <v>64</v>
+      </c>
+      <c r="C22">
+        <v>7</v>
+      </c>
+      <c r="D22">
+        <v>2.6717557251908302</v>
+      </c>
+      <c r="E22">
+        <v>2.4898758518937199E-2</v>
+      </c>
+      <c r="F22" t="s">
+        <v>65</v>
+      </c>
+      <c r="G22">
+        <v>213</v>
+      </c>
+      <c r="H22">
         <v>54</v>
       </c>
-      <c r="C22">
-        <v>3</v>
-      </c>
-      <c r="D22">
-        <v>1.3953488372092999</v>
-      </c>
-      <c r="E22">
-        <v>6.0255125141152902E-2</v>
-      </c>
-      <c r="F22" t="s">
-        <v>55</v>
-      </c>
-      <c r="G22">
-        <v>172</v>
-      </c>
-      <c r="H22">
-        <v>12</v>
-      </c>
       <c r="I22">
-        <v>5048</v>
+        <v>5033</v>
       </c>
       <c r="J22">
-        <v>7.3372093023255802</v>
+        <v>3.0630325160841498</v>
       </c>
       <c r="K22">
-        <v>1</v>
+        <v>0.99999999999719802</v>
       </c>
       <c r="L22">
         <v>1</v>
       </c>
-      <c r="M22">
-        <v>0.99649941656942798</v>
+      <c r="M22" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
@@ -1616,40 +2106,40 @@
         <v>13</v>
       </c>
       <c r="B23" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="C23">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D23">
-        <v>1.86046511627906</v>
+        <v>1.1450381679389301</v>
       </c>
       <c r="E23">
-        <v>6.1622375763307799E-2</v>
+        <v>3.2241555653194698E-2</v>
       </c>
       <c r="F23" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="G23">
-        <v>172</v>
+        <v>213</v>
       </c>
       <c r="H23">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="I23">
-        <v>5048</v>
+        <v>5033</v>
       </c>
       <c r="J23">
-        <v>4.3479758828595996</v>
+        <v>10.1267605633802</v>
       </c>
       <c r="K23">
-        <v>1</v>
+        <v>0.999999999999999</v>
       </c>
       <c r="L23">
         <v>1</v>
       </c>
-      <c r="M23">
-        <v>0.99649941656942798</v>
+      <c r="M23" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.2">
@@ -1657,31 +2147,31 @@
         <v>13</v>
       </c>
       <c r="B24" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="C24">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D24">
-        <v>2.3255813953488298</v>
+        <v>2.2900763358778602</v>
       </c>
       <c r="E24">
-        <v>6.4599663570688803E-2</v>
+        <v>3.61557731386805E-2</v>
       </c>
       <c r="F24" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="G24">
-        <v>172</v>
+        <v>213</v>
       </c>
       <c r="H24">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I24">
-        <v>5048</v>
+        <v>5033</v>
       </c>
       <c r="J24">
-        <v>3.2609819121446999</v>
+        <v>3.2221510883482698</v>
       </c>
       <c r="K24">
         <v>1</v>
@@ -1689,8 +2179,8 @@
       <c r="L24">
         <v>1</v>
       </c>
-      <c r="M24">
-        <v>0.99649941656942798</v>
+      <c r="M24" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.2">
@@ -1698,40 +2188,40 @@
         <v>13</v>
       </c>
       <c r="B25" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="C25">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D25">
-        <v>0.93023255813953398</v>
+        <v>1.90839694656488</v>
       </c>
       <c r="E25">
-        <v>6.6608586105782602E-2</v>
+        <v>3.9496651213476598E-2</v>
       </c>
       <c r="F25" t="s">
+        <v>71</v>
+      </c>
+      <c r="G25">
+        <v>213</v>
+      </c>
+      <c r="H25">
+        <v>31</v>
+      </c>
+      <c r="I25">
+        <v>5033</v>
+      </c>
+      <c r="J25">
+        <v>3.8111464485839699</v>
+      </c>
+      <c r="K25">
+        <v>1</v>
+      </c>
+      <c r="L25">
+        <v>1</v>
+      </c>
+      <c r="M25" t="s">
         <v>61</v>
-      </c>
-      <c r="G25">
-        <v>172</v>
-      </c>
-      <c r="H25">
-        <v>2</v>
-      </c>
-      <c r="I25">
-        <v>5048</v>
-      </c>
-      <c r="J25">
-        <v>29.3488372093023</v>
-      </c>
-      <c r="K25">
-        <v>1</v>
-      </c>
-      <c r="L25">
-        <v>1</v>
-      </c>
-      <c r="M25">
-        <v>0.99649941656942798</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.2">
@@ -1739,31 +2229,31 @@
         <v>13</v>
       </c>
       <c r="B26" t="s">
-        <v>62</v>
+        <v>72</v>
       </c>
       <c r="C26">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D26">
-        <v>0.93023255813953398</v>
+        <v>2.6717557251908302</v>
       </c>
       <c r="E26">
-        <v>6.6608586105782602E-2</v>
+        <v>4.2082345048120397E-2</v>
       </c>
       <c r="F26" t="s">
+        <v>73</v>
+      </c>
+      <c r="G26">
+        <v>213</v>
+      </c>
+      <c r="H26">
         <v>61</v>
       </c>
-      <c r="G26">
-        <v>172</v>
-      </c>
-      <c r="H26">
-        <v>2</v>
-      </c>
       <c r="I26">
-        <v>5048</v>
+        <v>5033</v>
       </c>
       <c r="J26">
-        <v>29.3488372093023</v>
+        <v>2.71153698145155</v>
       </c>
       <c r="K26">
         <v>1</v>
@@ -1771,8 +2261,8 @@
       <c r="L26">
         <v>1</v>
       </c>
-      <c r="M26">
-        <v>0.99649941656942798</v>
+      <c r="M26" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.2">
@@ -1780,31 +2270,31 @@
         <v>13</v>
       </c>
       <c r="B27" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="C27">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D27">
-        <v>0.93023255813953398</v>
+        <v>1.90839694656488</v>
       </c>
       <c r="E27">
-        <v>6.6608586105782602E-2</v>
+        <v>4.3702599826034499E-2</v>
       </c>
       <c r="F27" t="s">
-        <v>64</v>
+        <v>75</v>
       </c>
       <c r="G27">
-        <v>172</v>
+        <v>213</v>
       </c>
       <c r="H27">
-        <v>2</v>
+        <v>32</v>
       </c>
       <c r="I27">
-        <v>5048</v>
+        <v>5033</v>
       </c>
       <c r="J27">
-        <v>29.3488372093023</v>
+        <v>3.69204812206572</v>
       </c>
       <c r="K27">
         <v>1</v>
@@ -1812,8 +2302,8 @@
       <c r="L27">
         <v>1</v>
       </c>
-      <c r="M27">
-        <v>0.99649941656942798</v>
+      <c r="M27" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.2">
@@ -1821,31 +2311,31 @@
         <v>13</v>
       </c>
       <c r="B28" t="s">
-        <v>65</v>
+        <v>76</v>
       </c>
       <c r="C28">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D28">
-        <v>0.93023255813953398</v>
+        <v>2.2900763358778602</v>
       </c>
       <c r="E28">
-        <v>6.6608586105782602E-2</v>
+        <v>4.61898113843641E-2</v>
       </c>
       <c r="F28" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="G28">
-        <v>172</v>
+        <v>213</v>
       </c>
       <c r="H28">
-        <v>2</v>
+        <v>47</v>
       </c>
       <c r="I28">
-        <v>5048</v>
+        <v>5033</v>
       </c>
       <c r="J28">
-        <v>29.3488372093023</v>
+        <v>3.01648186994306</v>
       </c>
       <c r="K28">
         <v>1</v>
@@ -1853,8 +2343,8 @@
       <c r="L28">
         <v>1</v>
       </c>
-      <c r="M28">
-        <v>0.99649941656942798</v>
+      <c r="M28" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.2">
@@ -1862,40 +2352,40 @@
         <v>13</v>
       </c>
       <c r="B29" t="s">
-        <v>67</v>
+        <v>78</v>
       </c>
       <c r="C29">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D29">
-        <v>0.93023255813953398</v>
+        <v>1.5267175572519001</v>
       </c>
       <c r="E29">
-        <v>6.6608586105782602E-2</v>
+        <v>5.6029433673662102E-2</v>
       </c>
       <c r="F29" t="s">
+        <v>32</v>
+      </c>
+      <c r="G29">
+        <v>213</v>
+      </c>
+      <c r="H29">
+        <v>21</v>
+      </c>
+      <c r="I29">
+        <v>5033</v>
+      </c>
+      <c r="J29">
+        <v>4.5007824726134498</v>
+      </c>
+      <c r="K29">
+        <v>1</v>
+      </c>
+      <c r="L29">
+        <v>1</v>
+      </c>
+      <c r="M29" t="s">
         <v>61</v>
-      </c>
-      <c r="G29">
-        <v>172</v>
-      </c>
-      <c r="H29">
-        <v>2</v>
-      </c>
-      <c r="I29">
-        <v>5048</v>
-      </c>
-      <c r="J29">
-        <v>29.3488372093023</v>
-      </c>
-      <c r="K29">
-        <v>1</v>
-      </c>
-      <c r="L29">
-        <v>1</v>
-      </c>
-      <c r="M29">
-        <v>0.99649941656942798</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.2">
@@ -1903,31 +2393,31 @@
         <v>13</v>
       </c>
       <c r="B30" t="s">
-        <v>68</v>
+        <v>79</v>
       </c>
       <c r="C30">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D30">
-        <v>1.86046511627906</v>
+        <v>1.1450381679389301</v>
       </c>
       <c r="E30">
-        <v>6.7362694768034095E-2</v>
+        <v>6.3594462611955102E-2</v>
       </c>
       <c r="F30" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
       <c r="G30">
-        <v>172</v>
+        <v>213</v>
       </c>
       <c r="H30">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="I30">
-        <v>5048</v>
+        <v>5033</v>
       </c>
       <c r="J30">
-        <v>4.1926910299003302</v>
+        <v>7.0887323943661897</v>
       </c>
       <c r="K30">
         <v>1</v>
@@ -1935,8 +2425,8 @@
       <c r="L30">
         <v>1</v>
       </c>
-      <c r="M30">
-        <v>0.99649941656942798</v>
+      <c r="M30" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.2">
@@ -1944,31 +2434,31 @@
         <v>13</v>
       </c>
       <c r="B31" t="s">
-        <v>70</v>
+        <v>81</v>
       </c>
       <c r="C31">
         <v>3</v>
       </c>
       <c r="D31">
-        <v>1.3953488372092999</v>
+        <v>1.1450381679389301</v>
       </c>
       <c r="E31">
-        <v>6.9664699195392796E-2</v>
+        <v>6.3594462611955102E-2</v>
       </c>
       <c r="F31" t="s">
-        <v>71</v>
+        <v>82</v>
       </c>
       <c r="G31">
-        <v>172</v>
+        <v>213</v>
       </c>
       <c r="H31">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="I31">
-        <v>5048</v>
+        <v>5033</v>
       </c>
       <c r="J31">
-        <v>6.7728085867620704</v>
+        <v>7.0887323943661897</v>
       </c>
       <c r="K31">
         <v>1</v>
@@ -1976,8 +2466,8 @@
       <c r="L31">
         <v>1</v>
       </c>
-      <c r="M31">
-        <v>0.99649941656942798</v>
+      <c r="M31" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.2">
@@ -1985,31 +2475,31 @@
         <v>13</v>
       </c>
       <c r="B32" t="s">
-        <v>72</v>
+        <v>83</v>
       </c>
       <c r="C32">
         <v>3</v>
       </c>
       <c r="D32">
-        <v>1.3953488372092999</v>
+        <v>1.1450381679389301</v>
       </c>
       <c r="E32">
-        <v>7.9516252250229499E-2</v>
+        <v>7.5624322169995303E-2</v>
       </c>
       <c r="F32" t="s">
-        <v>73</v>
+        <v>84</v>
       </c>
       <c r="G32">
-        <v>172</v>
+        <v>213</v>
       </c>
       <c r="H32">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="I32">
-        <v>5048</v>
+        <v>5033</v>
       </c>
       <c r="J32">
-        <v>6.2890365448504904</v>
+        <v>6.4443021766965396</v>
       </c>
       <c r="K32">
         <v>1</v>
@@ -2017,8 +2507,8 @@
       <c r="L32">
         <v>1</v>
       </c>
-      <c r="M32">
-        <v>0.99649941656942798</v>
+      <c r="M32" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.2">
@@ -2026,31 +2516,31 @@
         <v>13</v>
       </c>
       <c r="B33" t="s">
-        <v>74</v>
+        <v>85</v>
       </c>
       <c r="C33">
         <v>5</v>
       </c>
       <c r="D33">
-        <v>2.3255813953488298</v>
+        <v>1.90839694656488</v>
       </c>
       <c r="E33">
-        <v>8.2943203159157597E-2</v>
+        <v>7.9833524494362595E-2</v>
       </c>
       <c r="F33" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="G33">
-        <v>172</v>
+        <v>213</v>
       </c>
       <c r="H33">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="I33">
-        <v>5048</v>
+        <v>5033</v>
       </c>
       <c r="J33">
-        <v>2.99477930707166</v>
+        <v>3.0293728181052102</v>
       </c>
       <c r="K33">
         <v>1</v>
@@ -2058,8 +2548,8 @@
       <c r="L33">
         <v>1</v>
       </c>
-      <c r="M33">
-        <v>0.99649941656942798</v>
+      <c r="M33" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.2">
@@ -2067,31 +2557,31 @@
         <v>13</v>
       </c>
       <c r="B34" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="C34">
         <v>2</v>
       </c>
       <c r="D34">
-        <v>0.93023255813953398</v>
+        <v>0.76335877862595403</v>
       </c>
       <c r="E34">
-        <v>9.8239567433038494E-2</v>
+        <v>8.2477745449216003E-2</v>
       </c>
       <c r="F34" t="s">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="G34">
-        <v>172</v>
+        <v>213</v>
       </c>
       <c r="H34">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I34">
-        <v>5048</v>
+        <v>5033</v>
       </c>
       <c r="J34">
-        <v>19.565891472868199</v>
+        <v>23.629107981220599</v>
       </c>
       <c r="K34">
         <v>1</v>
@@ -2099,8 +2589,8 @@
       <c r="L34">
         <v>1</v>
       </c>
-      <c r="M34">
-        <v>0.99649941656942798</v>
+      <c r="M34" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.2">
@@ -2108,31 +2598,31 @@
         <v>13</v>
       </c>
       <c r="B35" t="s">
-        <v>78</v>
+        <v>89</v>
       </c>
       <c r="C35">
         <v>2</v>
       </c>
       <c r="D35">
-        <v>0.93023255813953398</v>
+        <v>0.76335877862595403</v>
       </c>
       <c r="E35">
-        <v>9.8239567433038494E-2</v>
+        <v>8.2477745449216003E-2</v>
       </c>
       <c r="F35" t="s">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="G35">
-        <v>172</v>
+        <v>213</v>
       </c>
       <c r="H35">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I35">
-        <v>5048</v>
+        <v>5033</v>
       </c>
       <c r="J35">
-        <v>19.565891472868199</v>
+        <v>23.629107981220599</v>
       </c>
       <c r="K35">
         <v>1</v>
@@ -2140,8 +2630,8 @@
       <c r="L35">
         <v>1</v>
       </c>
-      <c r="M35">
-        <v>0.99649941656942798</v>
+      <c r="M35" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.2">
@@ -2149,31 +2639,31 @@
         <v>13</v>
       </c>
       <c r="B36" t="s">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="C36">
         <v>2</v>
       </c>
       <c r="D36">
-        <v>0.93023255813953398</v>
+        <v>0.76335877862595403</v>
       </c>
       <c r="E36">
-        <v>9.8239567433038494E-2</v>
+        <v>8.2477745449216003E-2</v>
       </c>
       <c r="F36" t="s">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="G36">
-        <v>172</v>
+        <v>213</v>
       </c>
       <c r="H36">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I36">
-        <v>5048</v>
+        <v>5033</v>
       </c>
       <c r="J36">
-        <v>19.565891472868199</v>
+        <v>23.629107981220599</v>
       </c>
       <c r="K36">
         <v>1</v>
@@ -2181,8 +2671,8 @@
       <c r="L36">
         <v>1</v>
       </c>
-      <c r="M36">
-        <v>0.99649941656942798</v>
+      <c r="M36" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.2">
@@ -2190,43 +2680,207 @@
         <v>13</v>
       </c>
       <c r="B37" t="s">
-        <v>82</v>
+        <v>93</v>
       </c>
       <c r="C37">
+        <v>2</v>
+      </c>
+      <c r="D37">
+        <v>0.76335877862595403</v>
+      </c>
+      <c r="E37">
+        <v>8.2477745449216003E-2</v>
+      </c>
+      <c r="F37" t="s">
+        <v>92</v>
+      </c>
+      <c r="G37">
+        <v>213</v>
+      </c>
+      <c r="H37">
+        <v>2</v>
+      </c>
+      <c r="I37">
+        <v>5033</v>
+      </c>
+      <c r="J37">
+        <v>23.629107981220599</v>
+      </c>
+      <c r="K37">
+        <v>1</v>
+      </c>
+      <c r="L37">
+        <v>1</v>
+      </c>
+      <c r="M37" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>13</v>
+      </c>
+      <c r="B38" t="s">
+        <v>94</v>
+      </c>
+      <c r="C38">
+        <v>2</v>
+      </c>
+      <c r="D38">
+        <v>0.76335877862595403</v>
+      </c>
+      <c r="E38">
+        <v>8.2477745449216003E-2</v>
+      </c>
+      <c r="F38" t="s">
+        <v>92</v>
+      </c>
+      <c r="G38">
+        <v>213</v>
+      </c>
+      <c r="H38">
+        <v>2</v>
+      </c>
+      <c r="I38">
+        <v>5033</v>
+      </c>
+      <c r="J38">
+        <v>23.629107981220599</v>
+      </c>
+      <c r="K38">
+        <v>1</v>
+      </c>
+      <c r="L38">
+        <v>1</v>
+      </c>
+      <c r="M38" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>13</v>
+      </c>
+      <c r="B39" t="s">
+        <v>95</v>
+      </c>
+      <c r="C39">
+        <v>2</v>
+      </c>
+      <c r="D39">
+        <v>0.76335877862595403</v>
+      </c>
+      <c r="E39">
+        <v>8.2477745449216003E-2</v>
+      </c>
+      <c r="F39" t="s">
+        <v>96</v>
+      </c>
+      <c r="G39">
+        <v>213</v>
+      </c>
+      <c r="H39">
+        <v>2</v>
+      </c>
+      <c r="I39">
+        <v>5033</v>
+      </c>
+      <c r="J39">
+        <v>23.629107981220599</v>
+      </c>
+      <c r="K39">
+        <v>1</v>
+      </c>
+      <c r="L39">
+        <v>1</v>
+      </c>
+      <c r="M39" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>13</v>
+      </c>
+      <c r="B40" t="s">
+        <v>97</v>
+      </c>
+      <c r="C40">
+        <v>3</v>
+      </c>
+      <c r="D40">
+        <v>1.1450381679389301</v>
+      </c>
+      <c r="E40">
+        <v>8.8303822889705896E-2</v>
+      </c>
+      <c r="F40" t="s">
+        <v>98</v>
+      </c>
+      <c r="G40">
+        <v>213</v>
+      </c>
+      <c r="H40">
+        <v>12</v>
+      </c>
+      <c r="I40">
+        <v>5033</v>
+      </c>
+      <c r="J40">
+        <v>5.9072769953051596</v>
+      </c>
+      <c r="K40">
+        <v>1</v>
+      </c>
+      <c r="L40">
+        <v>1</v>
+      </c>
+      <c r="M40" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>13</v>
+      </c>
+      <c r="B41" t="s">
+        <v>99</v>
+      </c>
+      <c r="C41">
         <v>4</v>
       </c>
-      <c r="D37">
-        <v>1.86046511627906</v>
-      </c>
-      <c r="E37">
-        <v>9.9441926841680003E-2</v>
-      </c>
-      <c r="F37" t="s">
-        <v>83</v>
-      </c>
-      <c r="G37">
-        <v>172</v>
-      </c>
-      <c r="H37">
-        <v>33</v>
-      </c>
-      <c r="I37">
-        <v>5048</v>
-      </c>
-      <c r="J37">
-        <v>3.5574348132487601</v>
-      </c>
-      <c r="K37">
-        <v>1</v>
-      </c>
-      <c r="L37">
-        <v>1</v>
-      </c>
-      <c r="M37">
-        <v>0.99649941656942798</v>
+      <c r="D41">
+        <v>1.5267175572519001</v>
+      </c>
+      <c r="E41">
+        <v>9.4143153362091003E-2</v>
+      </c>
+      <c r="F41" t="s">
+        <v>100</v>
+      </c>
+      <c r="G41">
+        <v>213</v>
+      </c>
+      <c r="H41">
+        <v>26</v>
+      </c>
+      <c r="I41">
+        <v>5033</v>
+      </c>
+      <c r="J41">
+        <v>3.6352473817262498</v>
+      </c>
+      <c r="K41">
+        <v>1</v>
+      </c>
+      <c r="L41">
+        <v>1</v>
+      </c>
+      <c r="M41" t="s">
+        <v>101</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>